<commit_message>
- CMD.04 -> CMD.06
</commit_message>
<xml_diff>
--- a/src/main/resources/data.xlsx
+++ b/src/main/resources/data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\java\SIEMENS\DesigoCCSpecifier_v5\src\main\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{16964690-DF6E-4DCE-BC85-63B3CE62BA75}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0BF9C09C-AB9D-4FA9-9FD7-D78635BBE82B}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-105" yWindow="-105" windowWidth="23250" windowHeight="12570" xr2:uid="{C2550A99-4CE5-415F-8594-E50E570FAC6E}"/>
   </bookViews>
@@ -2160,15 +2160,6 @@
     <t>AAC-16-GMS</t>
   </si>
   <si>
-    <t>S55802-Y148</t>
-  </si>
-  <si>
-    <t>CMD.04</t>
-  </si>
-  <si>
-    <t>ЭЛЕКТРОННЫЙ КЛЮЧ  LMS MICRO</t>
-  </si>
-  <si>
     <t>CMD.04 LMS Micro Dongle</t>
   </si>
   <si>
@@ -3090,13 +3081,22 @@
     <t>Desigo CC Удаленное оповещение</t>
   </si>
   <si>
-    <t>Модель данных: 29.12.2021</t>
-  </si>
-  <si>
     <t>Компонент продления подписки (SUR)</t>
   </si>
   <si>
     <t>Компонент возобновления подписки (SUS)</t>
+  </si>
+  <si>
+    <t>Модель данных: 26.01.2022</t>
+  </si>
+  <si>
+    <t>CMD.06</t>
+  </si>
+  <si>
+    <t>S55802-Y185</t>
+  </si>
+  <si>
+    <t>Электронный ключ LMS Micro</t>
   </si>
 </sst>
 </file>
@@ -3524,7 +3524,7 @@
   <dimension ref="A1:A2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G2" sqref="G2"/>
+      <selection activeCell="G5" sqref="G5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3534,12 +3534,12 @@
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>1015</v>
+        <v>1012</v>
       </c>
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
-        <v>1017</v>
+        <v>1016</v>
       </c>
     </row>
   </sheetData>
@@ -3579,10 +3579,10 @@
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>782</v>
+        <v>779</v>
       </c>
       <c r="B2" t="s">
-        <v>783</v>
+        <v>780</v>
       </c>
       <c r="C2">
         <v>1</v>
@@ -3593,10 +3593,10 @@
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>784</v>
+        <v>781</v>
       </c>
       <c r="B3" t="s">
-        <v>785</v>
+        <v>782</v>
       </c>
       <c r="C3">
         <v>8</v>
@@ -3607,10 +3607,10 @@
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>786</v>
+        <v>783</v>
       </c>
       <c r="B4" t="s">
-        <v>787</v>
+        <v>784</v>
       </c>
       <c r="C4">
         <v>8</v>
@@ -3663,10 +3663,10 @@
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>788</v>
+        <v>785</v>
       </c>
       <c r="B8" t="s">
-        <v>789</v>
+        <v>786</v>
       </c>
       <c r="C8">
         <v>1</v>
@@ -3677,10 +3677,10 @@
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>790</v>
+        <v>787</v>
       </c>
       <c r="B9" t="s">
-        <v>791</v>
+        <v>788</v>
       </c>
       <c r="C9">
         <v>1</v>
@@ -3719,10 +3719,10 @@
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>792</v>
+        <v>789</v>
       </c>
       <c r="B12" t="s">
-        <v>793</v>
+        <v>790</v>
       </c>
       <c r="C12">
         <v>1</v>
@@ -3747,10 +3747,10 @@
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>794</v>
+        <v>791</v>
       </c>
       <c r="B14" t="s">
-        <v>795</v>
+        <v>792</v>
       </c>
       <c r="C14">
         <v>1</v>
@@ -3761,10 +3761,10 @@
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>796</v>
+        <v>793</v>
       </c>
       <c r="B15" t="s">
-        <v>797</v>
+        <v>794</v>
       </c>
       <c r="C15">
         <v>1</v>
@@ -3775,10 +3775,10 @@
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>798</v>
+        <v>795</v>
       </c>
       <c r="B16" t="s">
-        <v>799</v>
+        <v>796</v>
       </c>
       <c r="C16">
         <v>1</v>
@@ -3789,10 +3789,10 @@
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>800</v>
+        <v>797</v>
       </c>
       <c r="B17" t="s">
-        <v>801</v>
+        <v>798</v>
       </c>
       <c r="C17">
         <v>1</v>
@@ -3803,10 +3803,10 @@
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>802</v>
+        <v>799</v>
       </c>
       <c r="B18" t="s">
-        <v>803</v>
+        <v>800</v>
       </c>
       <c r="C18">
         <v>1</v>
@@ -3845,10 +3845,10 @@
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>804</v>
+        <v>801</v>
       </c>
       <c r="B21" t="s">
-        <v>805</v>
+        <v>802</v>
       </c>
       <c r="C21">
         <v>3</v>
@@ -3873,10 +3873,10 @@
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>806</v>
+        <v>803</v>
       </c>
       <c r="B23" t="s">
-        <v>807</v>
+        <v>804</v>
       </c>
       <c r="C23">
         <v>3</v>
@@ -3887,10 +3887,10 @@
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>808</v>
+        <v>805</v>
       </c>
       <c r="B24" t="s">
-        <v>809</v>
+        <v>806</v>
       </c>
       <c r="C24">
         <v>1</v>
@@ -3901,10 +3901,10 @@
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>810</v>
+        <v>807</v>
       </c>
       <c r="B25" t="s">
-        <v>811</v>
+        <v>808</v>
       </c>
       <c r="C25">
         <v>1</v>
@@ -3915,10 +3915,10 @@
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>812</v>
+        <v>809</v>
       </c>
       <c r="B26" t="s">
-        <v>813</v>
+        <v>810</v>
       </c>
       <c r="C26">
         <v>1</v>
@@ -3929,10 +3929,10 @@
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>814</v>
+        <v>811</v>
       </c>
       <c r="B27" t="s">
-        <v>815</v>
+        <v>812</v>
       </c>
       <c r="C27">
         <v>1</v>
@@ -3943,10 +3943,10 @@
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>816</v>
+        <v>813</v>
       </c>
       <c r="B28" t="s">
-        <v>817</v>
+        <v>814</v>
       </c>
       <c r="C28">
         <v>1</v>
@@ -4013,10 +4013,10 @@
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>818</v>
+        <v>815</v>
       </c>
       <c r="B33" t="s">
-        <v>819</v>
+        <v>816</v>
       </c>
       <c r="C33">
         <v>1</v>
@@ -4027,10 +4027,10 @@
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>820</v>
+        <v>817</v>
       </c>
       <c r="B34" t="s">
-        <v>821</v>
+        <v>818</v>
       </c>
       <c r="C34">
         <v>1</v>
@@ -4041,10 +4041,10 @@
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>822</v>
+        <v>819</v>
       </c>
       <c r="B35" t="s">
-        <v>823</v>
+        <v>820</v>
       </c>
       <c r="C35">
         <v>1</v>
@@ -4083,10 +4083,10 @@
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>824</v>
+        <v>821</v>
       </c>
       <c r="B38" t="s">
-        <v>825</v>
+        <v>822</v>
       </c>
       <c r="C38">
         <v>1</v>
@@ -4111,10 +4111,10 @@
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>826</v>
+        <v>823</v>
       </c>
       <c r="B40" t="s">
-        <v>827</v>
+        <v>824</v>
       </c>
       <c r="C40">
         <v>1</v>
@@ -4125,10 +4125,10 @@
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
-        <v>828</v>
+        <v>825</v>
       </c>
       <c r="B41" t="s">
-        <v>829</v>
+        <v>826</v>
       </c>
       <c r="C41">
         <v>8</v>
@@ -4139,10 +4139,10 @@
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
-        <v>830</v>
+        <v>827</v>
       </c>
       <c r="B42" t="s">
-        <v>831</v>
+        <v>828</v>
       </c>
       <c r="C42">
         <v>1</v>
@@ -4153,10 +4153,10 @@
     </row>
     <row r="43" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
-        <v>832</v>
+        <v>829</v>
       </c>
       <c r="B43" t="s">
-        <v>833</v>
+        <v>830</v>
       </c>
       <c r="C43">
         <v>1</v>
@@ -4167,10 +4167,10 @@
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
-        <v>834</v>
+        <v>831</v>
       </c>
       <c r="B44" t="s">
-        <v>835</v>
+        <v>832</v>
       </c>
       <c r="C44">
         <v>1</v>
@@ -4181,10 +4181,10 @@
     </row>
     <row r="45" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
-        <v>836</v>
+        <v>833</v>
       </c>
       <c r="B45" t="s">
-        <v>837</v>
+        <v>834</v>
       </c>
       <c r="C45">
         <v>40</v>
@@ -4237,10 +4237,10 @@
     </row>
     <row r="49" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
-        <v>838</v>
+        <v>835</v>
       </c>
       <c r="B49" t="s">
-        <v>839</v>
+        <v>836</v>
       </c>
       <c r="C49">
         <v>1</v>
@@ -4335,10 +4335,10 @@
     </row>
     <row r="56" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
-        <v>840</v>
+        <v>837</v>
       </c>
       <c r="B56" t="s">
-        <v>841</v>
+        <v>838</v>
       </c>
       <c r="C56">
         <v>1</v>
@@ -4363,10 +4363,10 @@
     </row>
     <row r="58" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
-        <v>842</v>
+        <v>839</v>
       </c>
       <c r="B58" t="s">
-        <v>843</v>
+        <v>840</v>
       </c>
       <c r="C58">
         <v>1</v>
@@ -4377,10 +4377,10 @@
     </row>
     <row r="59" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
-        <v>844</v>
+        <v>841</v>
       </c>
       <c r="B59" t="s">
-        <v>845</v>
+        <v>842</v>
       </c>
       <c r="C59">
         <v>1</v>
@@ -4405,10 +4405,10 @@
     </row>
     <row r="61" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
-        <v>846</v>
+        <v>843</v>
       </c>
       <c r="B61" t="s">
-        <v>847</v>
+        <v>844</v>
       </c>
       <c r="C61">
         <v>1</v>
@@ -4447,10 +4447,10 @@
     </row>
     <row r="64" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
-        <v>848</v>
+        <v>845</v>
       </c>
       <c r="B64" t="s">
-        <v>849</v>
+        <v>846</v>
       </c>
       <c r="C64">
         <v>1</v>
@@ -4475,10 +4475,10 @@
     </row>
     <row r="66" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
-        <v>850</v>
+        <v>847</v>
       </c>
       <c r="B66" t="s">
-        <v>851</v>
+        <v>848</v>
       </c>
       <c r="C66">
         <v>1</v>
@@ -4489,10 +4489,10 @@
     </row>
     <row r="67" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
-        <v>852</v>
+        <v>849</v>
       </c>
       <c r="B67" t="s">
-        <v>853</v>
+        <v>850</v>
       </c>
       <c r="C67">
         <v>1</v>
@@ -4503,10 +4503,10 @@
     </row>
     <row r="68" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
-        <v>854</v>
+        <v>851</v>
       </c>
       <c r="B68" t="s">
-        <v>855</v>
+        <v>852</v>
       </c>
       <c r="C68">
         <v>1</v>
@@ -4517,10 +4517,10 @@
     </row>
     <row r="69" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
-        <v>856</v>
+        <v>853</v>
       </c>
       <c r="B69" t="s">
-        <v>857</v>
+        <v>854</v>
       </c>
       <c r="C69">
         <v>1</v>
@@ -4531,10 +4531,10 @@
     </row>
     <row r="70" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
-        <v>858</v>
+        <v>855</v>
       </c>
       <c r="B70" t="s">
-        <v>859</v>
+        <v>856</v>
       </c>
       <c r="C70">
         <v>1</v>
@@ -4545,10 +4545,10 @@
     </row>
     <row r="71" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
-        <v>860</v>
+        <v>857</v>
       </c>
       <c r="B71" t="s">
-        <v>861</v>
+        <v>858</v>
       </c>
       <c r="C71">
         <v>1</v>
@@ -4559,10 +4559,10 @@
     </row>
     <row r="72" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
-        <v>862</v>
+        <v>859</v>
       </c>
       <c r="B72" t="s">
-        <v>863</v>
+        <v>860</v>
       </c>
       <c r="C72">
         <v>1</v>
@@ -4573,10 +4573,10 @@
     </row>
     <row r="73" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
-        <v>864</v>
+        <v>861</v>
       </c>
       <c r="B73" t="s">
-        <v>865</v>
+        <v>862</v>
       </c>
       <c r="C73">
         <v>1</v>
@@ -4587,10 +4587,10 @@
     </row>
     <row r="74" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
-        <v>866</v>
+        <v>863</v>
       </c>
       <c r="B74" t="s">
-        <v>867</v>
+        <v>864</v>
       </c>
       <c r="C74">
         <v>1</v>
@@ -4601,10 +4601,10 @@
     </row>
     <row r="75" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
-        <v>868</v>
+        <v>865</v>
       </c>
       <c r="B75" t="s">
-        <v>869</v>
+        <v>866</v>
       </c>
       <c r="C75">
         <v>1</v>
@@ -4615,10 +4615,10 @@
     </row>
     <row r="76" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A76" t="s">
-        <v>870</v>
+        <v>867</v>
       </c>
       <c r="B76" t="s">
-        <v>871</v>
+        <v>868</v>
       </c>
       <c r="C76">
         <v>1</v>
@@ -4643,10 +4643,10 @@
     </row>
     <row r="78" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A78" t="s">
-        <v>872</v>
+        <v>869</v>
       </c>
       <c r="B78" t="s">
-        <v>873</v>
+        <v>870</v>
       </c>
       <c r="C78">
         <v>1</v>
@@ -4657,10 +4657,10 @@
     </row>
     <row r="79" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A79" t="s">
-        <v>874</v>
+        <v>871</v>
       </c>
       <c r="B79" t="s">
-        <v>875</v>
+        <v>872</v>
       </c>
       <c r="C79">
         <v>1</v>
@@ -4685,10 +4685,10 @@
     </row>
     <row r="81" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A81" t="s">
-        <v>876</v>
+        <v>873</v>
       </c>
       <c r="B81" t="s">
-        <v>877</v>
+        <v>874</v>
       </c>
       <c r="C81">
         <v>1</v>
@@ -4699,10 +4699,10 @@
     </row>
     <row r="82" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A82" t="s">
-        <v>878</v>
+        <v>875</v>
       </c>
       <c r="B82" t="s">
-        <v>879</v>
+        <v>876</v>
       </c>
       <c r="C82">
         <v>1</v>
@@ -4727,10 +4727,10 @@
     </row>
     <row r="84" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A84" t="s">
-        <v>880</v>
+        <v>877</v>
       </c>
       <c r="B84" t="s">
-        <v>881</v>
+        <v>878</v>
       </c>
       <c r="C84">
         <v>0</v>
@@ -4741,10 +4741,10 @@
     </row>
     <row r="85" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A85" t="s">
-        <v>882</v>
+        <v>879</v>
       </c>
       <c r="B85" t="s">
-        <v>883</v>
+        <v>880</v>
       </c>
       <c r="C85">
         <v>10</v>
@@ -4755,10 +4755,10 @@
     </row>
     <row r="86" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A86" t="s">
-        <v>884</v>
+        <v>881</v>
       </c>
       <c r="B86" t="s">
-        <v>885</v>
+        <v>882</v>
       </c>
       <c r="C86">
         <v>10</v>
@@ -4825,10 +4825,10 @@
     </row>
     <row r="91" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A91" t="s">
-        <v>886</v>
+        <v>883</v>
       </c>
       <c r="B91" t="s">
-        <v>887</v>
+        <v>884</v>
       </c>
       <c r="C91">
         <v>15</v>
@@ -4839,10 +4839,10 @@
     </row>
     <row r="92" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A92" t="s">
-        <v>888</v>
+        <v>885</v>
       </c>
       <c r="B92" t="s">
-        <v>889</v>
+        <v>886</v>
       </c>
       <c r="C92">
         <v>15</v>
@@ -4853,10 +4853,10 @@
     </row>
     <row r="93" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A93" t="s">
-        <v>890</v>
+        <v>887</v>
       </c>
       <c r="B93" t="s">
-        <v>891</v>
+        <v>888</v>
       </c>
       <c r="C93">
         <v>15</v>
@@ -4867,10 +4867,10 @@
     </row>
     <row r="94" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A94" t="s">
-        <v>892</v>
+        <v>889</v>
       </c>
       <c r="B94" t="s">
-        <v>893</v>
+        <v>890</v>
       </c>
       <c r="C94">
         <v>15</v>
@@ -4909,10 +4909,10 @@
     </row>
     <row r="97" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A97" t="s">
-        <v>894</v>
+        <v>891</v>
       </c>
       <c r="B97" t="s">
-        <v>895</v>
+        <v>892</v>
       </c>
       <c r="C97">
         <v>20</v>
@@ -4923,10 +4923,10 @@
     </row>
     <row r="98" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A98" t="s">
-        <v>896</v>
+        <v>893</v>
       </c>
       <c r="B98" t="s">
-        <v>897</v>
+        <v>894</v>
       </c>
       <c r="C98">
         <v>20</v>
@@ -4937,10 +4937,10 @@
     </row>
     <row r="99" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A99" t="s">
-        <v>898</v>
+        <v>895</v>
       </c>
       <c r="B99" t="s">
-        <v>899</v>
+        <v>896</v>
       </c>
       <c r="C99">
         <v>20</v>
@@ -4979,10 +4979,10 @@
     </row>
     <row r="102" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A102" t="s">
-        <v>900</v>
+        <v>897</v>
       </c>
       <c r="B102" t="s">
-        <v>901</v>
+        <v>898</v>
       </c>
       <c r="C102">
         <v>20</v>
@@ -4993,10 +4993,10 @@
     </row>
     <row r="103" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A103" t="s">
-        <v>902</v>
+        <v>899</v>
       </c>
       <c r="B103" t="s">
-        <v>903</v>
+        <v>900</v>
       </c>
       <c r="C103">
         <v>15</v>
@@ -5007,10 +5007,10 @@
     </row>
     <row r="104" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A104" t="s">
-        <v>904</v>
+        <v>901</v>
       </c>
       <c r="B104" t="s">
-        <v>905</v>
+        <v>902</v>
       </c>
       <c r="C104">
         <v>8</v>
@@ -5063,10 +5063,10 @@
     </row>
     <row r="108" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A108" t="s">
-        <v>906</v>
+        <v>903</v>
       </c>
       <c r="B108" t="s">
-        <v>907</v>
+        <v>904</v>
       </c>
       <c r="C108">
         <v>40</v>
@@ -5077,10 +5077,10 @@
     </row>
     <row r="109" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A109" t="s">
-        <v>908</v>
+        <v>905</v>
       </c>
       <c r="B109" t="s">
-        <v>909</v>
+        <v>906</v>
       </c>
       <c r="C109">
         <v>1</v>
@@ -5091,10 +5091,10 @@
     </row>
     <row r="110" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A110" t="s">
-        <v>910</v>
+        <v>907</v>
       </c>
       <c r="B110" t="s">
-        <v>911</v>
+        <v>908</v>
       </c>
       <c r="C110">
         <v>1</v>
@@ -5105,10 +5105,10 @@
     </row>
     <row r="111" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A111" t="s">
-        <v>912</v>
+        <v>909</v>
       </c>
       <c r="B111" t="s">
-        <v>913</v>
+        <v>910</v>
       </c>
       <c r="C111">
         <v>1</v>
@@ -5119,10 +5119,10 @@
     </row>
     <row r="112" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A112" t="s">
-        <v>914</v>
+        <v>911</v>
       </c>
       <c r="B112" t="s">
-        <v>915</v>
+        <v>912</v>
       </c>
       <c r="C112">
         <v>1</v>
@@ -5133,10 +5133,10 @@
     </row>
     <row r="113" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A113" t="s">
-        <v>916</v>
+        <v>913</v>
       </c>
       <c r="B113" t="s">
-        <v>917</v>
+        <v>914</v>
       </c>
       <c r="C113">
         <v>4</v>
@@ -5189,10 +5189,10 @@
     </row>
     <row r="117" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A117" t="s">
-        <v>918</v>
+        <v>915</v>
       </c>
       <c r="B117" t="s">
-        <v>919</v>
+        <v>916</v>
       </c>
       <c r="C117">
         <v>1</v>
@@ -5203,10 +5203,10 @@
     </row>
     <row r="118" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A118" t="s">
-        <v>920</v>
+        <v>917</v>
       </c>
       <c r="B118" t="s">
-        <v>921</v>
+        <v>918</v>
       </c>
       <c r="C118">
         <v>1</v>
@@ -5217,10 +5217,10 @@
     </row>
     <row r="119" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A119" t="s">
-        <v>922</v>
+        <v>919</v>
       </c>
       <c r="B119" t="s">
-        <v>923</v>
+        <v>920</v>
       </c>
       <c r="C119">
         <v>1</v>
@@ -5231,10 +5231,10 @@
     </row>
     <row r="120" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A120" t="s">
-        <v>924</v>
+        <v>921</v>
       </c>
       <c r="B120" t="s">
-        <v>925</v>
+        <v>922</v>
       </c>
       <c r="C120">
         <v>1</v>
@@ -5281,10 +5281,10 @@
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>926</v>
+        <v>923</v>
       </c>
       <c r="B2" t="s">
-        <v>927</v>
+        <v>924</v>
       </c>
       <c r="C2">
         <v>30</v>
@@ -5295,10 +5295,10 @@
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>928</v>
+        <v>925</v>
       </c>
       <c r="B3" t="s">
-        <v>929</v>
+        <v>926</v>
       </c>
       <c r="C3">
         <v>2</v>
@@ -5309,10 +5309,10 @@
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>930</v>
+        <v>927</v>
       </c>
       <c r="B4" t="s">
-        <v>931</v>
+        <v>928</v>
       </c>
       <c r="C4">
         <v>2</v>
@@ -5323,10 +5323,10 @@
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>932</v>
+        <v>929</v>
       </c>
       <c r="B5" t="s">
-        <v>933</v>
+        <v>930</v>
       </c>
       <c r="C5">
         <v>26</v>
@@ -5337,10 +5337,10 @@
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>934</v>
+        <v>931</v>
       </c>
       <c r="B6" t="s">
-        <v>935</v>
+        <v>932</v>
       </c>
       <c r="C6">
         <v>4</v>
@@ -5351,10 +5351,10 @@
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>936</v>
+        <v>933</v>
       </c>
       <c r="B7" t="s">
-        <v>937</v>
+        <v>934</v>
       </c>
       <c r="C7">
         <v>8</v>
@@ -5365,10 +5365,10 @@
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>938</v>
+        <v>935</v>
       </c>
       <c r="B8" t="s">
-        <v>939</v>
+        <v>936</v>
       </c>
       <c r="C8">
         <v>20</v>
@@ -5379,10 +5379,10 @@
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>940</v>
+        <v>937</v>
       </c>
       <c r="B9" t="s">
-        <v>941</v>
+        <v>938</v>
       </c>
       <c r="C9">
         <v>42</v>
@@ -5393,10 +5393,10 @@
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>942</v>
+        <v>939</v>
       </c>
       <c r="B10" t="s">
-        <v>943</v>
+        <v>940</v>
       </c>
       <c r="C10">
         <v>2</v>
@@ -5407,10 +5407,10 @@
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>944</v>
+        <v>941</v>
       </c>
       <c r="B11" t="s">
-        <v>945</v>
+        <v>942</v>
       </c>
       <c r="C11">
         <v>1</v>
@@ -5421,10 +5421,10 @@
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>946</v>
+        <v>943</v>
       </c>
       <c r="B12" t="s">
-        <v>947</v>
+        <v>944</v>
       </c>
       <c r="C12">
         <v>21</v>
@@ -5435,10 +5435,10 @@
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>948</v>
+        <v>945</v>
       </c>
       <c r="B13" t="s">
-        <v>949</v>
+        <v>946</v>
       </c>
       <c r="C13">
         <v>24</v>
@@ -5449,10 +5449,10 @@
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>950</v>
+        <v>947</v>
       </c>
       <c r="B14" t="s">
-        <v>951</v>
+        <v>948</v>
       </c>
       <c r="C14">
         <v>1</v>
@@ -6097,7 +6097,7 @@
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>990</v>
+        <v>987</v>
       </c>
       <c r="B2" t="s">
         <v>28</v>
@@ -6182,7 +6182,7 @@
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>718</v>
+        <v>715</v>
       </c>
       <c r="B10" t="s">
         <v>42</v>
@@ -6193,7 +6193,7 @@
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>717</v>
+        <v>714</v>
       </c>
       <c r="B11" t="s">
         <v>43</v>
@@ -6204,13 +6204,13 @@
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>735</v>
+        <v>732</v>
       </c>
       <c r="B12" t="s">
-        <v>734</v>
+        <v>731</v>
       </c>
       <c r="C12" t="s">
-        <v>734</v>
+        <v>731</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
@@ -6248,24 +6248,24 @@
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>1018</v>
+        <v>1014</v>
       </c>
       <c r="B16" t="s">
-        <v>985</v>
+        <v>982</v>
       </c>
       <c r="C16" t="s">
-        <v>985</v>
+        <v>982</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>1019</v>
+        <v>1015</v>
       </c>
       <c r="B17" t="s">
-        <v>986</v>
+        <v>983</v>
       </c>
       <c r="C17" t="s">
-        <v>986</v>
+        <v>983</v>
       </c>
     </row>
   </sheetData>
@@ -6326,24 +6326,24 @@
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>958</v>
+        <v>955</v>
       </c>
       <c r="B7" t="s">
-        <v>993</v>
+        <v>990</v>
       </c>
       <c r="C7" t="s">
-        <v>994</v>
+        <v>991</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>953</v>
+        <v>950</v>
       </c>
       <c r="B8" t="s">
-        <v>952</v>
+        <v>949</v>
       </c>
       <c r="C8" t="s">
-        <v>954</v>
+        <v>951</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
@@ -6358,7 +6358,7 @@
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>955</v>
+        <v>952</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
@@ -6394,7 +6394,7 @@
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>956</v>
+        <v>953</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.25">
@@ -6404,23 +6404,23 @@
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>957</v>
+        <v>954</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>989</v>
+        <v>986</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>723</v>
+        <v>720</v>
       </c>
       <c r="B21" t="s">
-        <v>724</v>
+        <v>721</v>
       </c>
       <c r="C21" t="s">
-        <v>725</v>
+        <v>722</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.25">
@@ -6444,7 +6444,7 @@
   <dimension ref="A1:H8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="H15" sqref="H15"/>
+      <selection activeCell="E19" sqref="E19:E20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6472,13 +6472,13 @@
         <v>705</v>
       </c>
       <c r="F1" s="7" t="s">
-        <v>712</v>
+        <v>709</v>
       </c>
       <c r="G1" s="7" t="s">
+        <v>710</v>
+      </c>
+      <c r="H1" s="8" t="s">
         <v>713</v>
-      </c>
-      <c r="H1" s="8" t="s">
-        <v>716</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
@@ -6489,22 +6489,22 @@
         <v>542</v>
       </c>
       <c r="C2" t="s">
-        <v>722</v>
+        <v>719</v>
       </c>
       <c r="D2" s="3" t="s">
         <v>60</v>
       </c>
       <c r="E2" t="s">
-        <v>708</v>
+        <v>1017</v>
       </c>
       <c r="F2" t="s">
-        <v>715</v>
+        <v>712</v>
       </c>
       <c r="G2" t="s">
-        <v>715</v>
+        <v>712</v>
       </c>
       <c r="H2" t="s">
-        <v>715</v>
+        <v>712</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
@@ -6515,44 +6515,44 @@
         <v>55</v>
       </c>
       <c r="C3" t="s">
-        <v>730</v>
+        <v>727</v>
       </c>
       <c r="D3" s="3"/>
       <c r="E3" t="s">
-        <v>708</v>
+        <v>1017</v>
       </c>
       <c r="F3" t="s">
-        <v>715</v>
+        <v>712</v>
       </c>
       <c r="G3" t="s">
-        <v>714</v>
+        <v>711</v>
       </c>
       <c r="H3" t="s">
-        <v>715</v>
+        <v>712</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>995</v>
+        <v>992</v>
       </c>
       <c r="B4" t="s">
-        <v>996</v>
+        <v>993</v>
       </c>
       <c r="C4" t="s">
-        <v>997</v>
+        <v>994</v>
       </c>
       <c r="D4" s="3"/>
       <c r="E4" t="s">
-        <v>708</v>
+        <v>1017</v>
       </c>
       <c r="F4" t="s">
-        <v>715</v>
+        <v>712</v>
       </c>
       <c r="G4" t="s">
-        <v>714</v>
+        <v>711</v>
       </c>
       <c r="H4" t="s">
-        <v>715</v>
+        <v>712</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
@@ -6563,20 +6563,20 @@
         <v>56</v>
       </c>
       <c r="C5" t="s">
-        <v>729</v>
+        <v>726</v>
       </c>
       <c r="D5" s="3"/>
       <c r="E5" t="s">
-        <v>708</v>
+        <v>1017</v>
       </c>
       <c r="F5" t="s">
-        <v>715</v>
+        <v>712</v>
       </c>
       <c r="G5" t="s">
-        <v>715</v>
+        <v>712</v>
       </c>
       <c r="H5" t="s">
-        <v>715</v>
+        <v>712</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.25">
@@ -6587,44 +6587,44 @@
         <v>57</v>
       </c>
       <c r="C6" t="s">
-        <v>728</v>
+        <v>725</v>
       </c>
       <c r="D6" s="3"/>
       <c r="E6" t="s">
-        <v>708</v>
+        <v>1017</v>
       </c>
       <c r="F6" t="s">
-        <v>714</v>
+        <v>711</v>
       </c>
       <c r="G6" t="s">
-        <v>714</v>
+        <v>711</v>
       </c>
       <c r="H6" t="s">
-        <v>715</v>
+        <v>712</v>
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>732</v>
+        <v>729</v>
       </c>
       <c r="B7" t="s">
-        <v>733</v>
+        <v>730</v>
       </c>
       <c r="C7" t="s">
-        <v>727</v>
+        <v>724</v>
       </c>
       <c r="D7" s="3"/>
       <c r="E7" t="s">
-        <v>708</v>
+        <v>1017</v>
       </c>
       <c r="F7" t="s">
-        <v>714</v>
+        <v>711</v>
       </c>
       <c r="G7" t="s">
-        <v>714</v>
+        <v>711</v>
       </c>
       <c r="H7" t="s">
-        <v>715</v>
+        <v>712</v>
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.25">
@@ -6635,20 +6635,20 @@
         <v>58</v>
       </c>
       <c r="C8" t="s">
-        <v>731</v>
+        <v>728</v>
       </c>
       <c r="D8" s="3"/>
       <c r="E8" t="s">
-        <v>708</v>
+        <v>1017</v>
       </c>
       <c r="F8" t="s">
-        <v>715</v>
+        <v>712</v>
       </c>
       <c r="G8" t="s">
-        <v>715</v>
+        <v>712</v>
       </c>
       <c r="H8" t="s">
-        <v>715</v>
+        <v>712</v>
       </c>
     </row>
   </sheetData>
@@ -6663,7 +6663,7 @@
   <dimension ref="A1:O17"/>
   <sheetViews>
     <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="G3" sqref="G3"/>
+      <selection activeCell="H8" sqref="H8:I8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7382,7 +7382,7 @@
     </row>
     <row r="16" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>987</v>
+        <v>984</v>
       </c>
       <c r="B16" s="14">
         <v>0</v>
@@ -7429,7 +7429,7 @@
     </row>
     <row r="17" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>988</v>
+        <v>985</v>
       </c>
       <c r="B17" s="14">
         <v>0</v>
@@ -8027,7 +8027,7 @@
     </row>
     <row r="20" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>989</v>
+        <v>986</v>
       </c>
       <c r="B20" s="14">
         <v>1</v>
@@ -8142,7 +8142,7 @@
   <dimension ref="A1:C3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F24" sqref="F24"/>
+      <selection activeCell="C18" sqref="C18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -8154,35 +8154,35 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>719</v>
+        <v>716</v>
       </c>
       <c r="B1" t="s">
         <v>591</v>
       </c>
       <c r="C1" t="s">
-        <v>720</v>
+        <v>717</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>721</v>
+        <v>718</v>
       </c>
       <c r="B2" t="s">
         <v>219</v>
       </c>
       <c r="C2" t="s">
-        <v>715</v>
+        <v>712</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>721</v>
+        <v>718</v>
       </c>
       <c r="B3" t="s">
-        <v>708</v>
+        <v>1017</v>
       </c>
       <c r="C3" t="s">
-        <v>715</v>
+        <v>712</v>
       </c>
     </row>
   </sheetData>
@@ -8194,8 +8194,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{23746BB9-1DD0-4EAB-8A33-BFEF932BE348}">
   <dimension ref="A1:E146"/>
   <sheetViews>
-    <sheetView topLeftCell="A124" workbookViewId="0">
-      <selection activeCell="C131" sqref="C131"/>
+    <sheetView topLeftCell="A115" workbookViewId="0">
+      <selection activeCell="C127" sqref="C127"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -10296,16 +10296,16 @@
     </row>
     <row r="124" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A124" t="s">
+        <v>1018</v>
+      </c>
+      <c r="B124" t="s">
+        <v>1017</v>
+      </c>
+      <c r="C124" t="s">
         <v>707</v>
       </c>
-      <c r="B124" t="s">
-        <v>708</v>
-      </c>
-      <c r="C124" t="s">
-        <v>710</v>
-      </c>
       <c r="D124" t="s">
-        <v>709</v>
+        <v>1019</v>
       </c>
       <c r="E124" s="13">
         <v>271</v>
@@ -10313,28 +10313,28 @@
     </row>
     <row r="125" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A125" t="s">
-        <v>991</v>
+        <v>988</v>
       </c>
       <c r="B125" t="s">
         <v>706</v>
       </c>
       <c r="C125" t="s">
-        <v>711</v>
+        <v>708</v>
       </c>
       <c r="D125" t="s">
-        <v>992</v>
+        <v>989</v>
       </c>
       <c r="E125" s="13"/>
     </row>
     <row r="126" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A126" s="12" t="s">
-        <v>959</v>
+        <v>956</v>
       </c>
       <c r="B126" s="12" t="s">
-        <v>960</v>
+        <v>957</v>
       </c>
       <c r="D126" s="12" t="s">
-        <v>961</v>
+        <v>958</v>
       </c>
       <c r="E126" s="13">
         <v>59600</v>
@@ -10342,13 +10342,13 @@
     </row>
     <row r="127" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A127" s="12" t="s">
-        <v>962</v>
+        <v>959</v>
       </c>
       <c r="B127" s="12" t="s">
-        <v>963</v>
+        <v>960</v>
       </c>
       <c r="D127" s="12" t="s">
-        <v>964</v>
+        <v>961</v>
       </c>
       <c r="E127" s="13">
         <v>29800</v>
@@ -10356,13 +10356,13 @@
     </row>
     <row r="128" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A128" s="12" t="s">
-        <v>736</v>
+        <v>733</v>
       </c>
       <c r="B128" s="12" t="s">
+        <v>734</v>
+      </c>
+      <c r="D128" s="12" t="s">
         <v>737</v>
-      </c>
-      <c r="D128" s="12" t="s">
-        <v>740</v>
       </c>
       <c r="E128" s="13">
         <v>1150</v>
@@ -10370,13 +10370,13 @@
     </row>
     <row r="129" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A129" s="12" t="s">
+        <v>735</v>
+      </c>
+      <c r="B129" s="12" t="s">
+        <v>736</v>
+      </c>
+      <c r="D129" s="12" t="s">
         <v>738</v>
-      </c>
-      <c r="B129" s="12" t="s">
-        <v>739</v>
-      </c>
-      <c r="D129" s="12" t="s">
-        <v>741</v>
       </c>
       <c r="E129" s="13">
         <v>8990</v>
@@ -10384,13 +10384,13 @@
     </row>
     <row r="130" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A130" s="12" t="s">
-        <v>742</v>
+        <v>739</v>
       </c>
       <c r="B130" s="12" t="s">
-        <v>732</v>
+        <v>729</v>
       </c>
       <c r="D130" s="12" t="s">
-        <v>743</v>
+        <v>740</v>
       </c>
       <c r="E130" s="13">
         <v>2990</v>
@@ -10398,13 +10398,13 @@
     </row>
     <row r="131" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A131" s="10" t="s">
-        <v>780</v>
+        <v>777</v>
       </c>
       <c r="B131" t="s">
-        <v>776</v>
+        <v>773</v>
       </c>
       <c r="D131" t="s">
-        <v>777</v>
+        <v>774</v>
       </c>
       <c r="E131" s="13">
         <v>5314.4</v>
@@ -10412,13 +10412,13 @@
     </row>
     <row r="132" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A132" s="10" t="s">
-        <v>781</v>
+        <v>778</v>
       </c>
       <c r="B132" t="s">
-        <v>778</v>
+        <v>775</v>
       </c>
       <c r="D132" t="s">
-        <v>779</v>
+        <v>776</v>
       </c>
       <c r="E132" s="13">
         <v>1410.36</v>
@@ -10426,104 +10426,104 @@
     </row>
     <row r="133" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A133" s="12" t="s">
-        <v>965</v>
+        <v>962</v>
       </c>
       <c r="B133" s="12" t="s">
-        <v>966</v>
+        <v>963</v>
       </c>
       <c r="C133" s="12" t="s">
-        <v>977</v>
+        <v>974</v>
       </c>
       <c r="D133" s="12" t="s">
-        <v>978</v>
+        <v>975</v>
       </c>
       <c r="E133" s="13"/>
     </row>
     <row r="134" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A134" s="12" t="s">
-        <v>967</v>
+        <v>964</v>
       </c>
       <c r="B134" s="12" t="s">
-        <v>968</v>
+        <v>965</v>
       </c>
       <c r="C134" s="12" t="s">
-        <v>979</v>
+        <v>976</v>
       </c>
       <c r="D134" s="12" t="s">
-        <v>980</v>
+        <v>977</v>
       </c>
       <c r="E134" s="13"/>
     </row>
     <row r="135" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A135" s="12" t="s">
-        <v>969</v>
+        <v>966</v>
       </c>
       <c r="B135" s="12" t="s">
-        <v>970</v>
+        <v>967</v>
       </c>
       <c r="C135" s="12" t="s">
-        <v>981</v>
+        <v>978</v>
       </c>
       <c r="D135" s="12" t="s">
-        <v>971</v>
+        <v>968</v>
       </c>
       <c r="E135" s="13"/>
     </row>
     <row r="136" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A136" s="12" t="s">
-        <v>972</v>
+        <v>969</v>
       </c>
       <c r="B136" s="12" t="s">
-        <v>954</v>
+        <v>951</v>
       </c>
       <c r="C136" s="12" t="s">
-        <v>982</v>
+        <v>979</v>
       </c>
       <c r="D136" s="12" t="s">
-        <v>973</v>
+        <v>970</v>
       </c>
       <c r="E136" s="13"/>
     </row>
     <row r="137" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A137" s="12" t="s">
-        <v>974</v>
+        <v>971</v>
       </c>
       <c r="B137" s="12" t="s">
-        <v>975</v>
+        <v>972</v>
       </c>
       <c r="C137" s="12" t="s">
-        <v>983</v>
+        <v>980</v>
       </c>
       <c r="D137" s="12" t="s">
-        <v>976</v>
+        <v>973</v>
       </c>
       <c r="E137" s="13"/>
     </row>
     <row r="138" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A138" s="12" t="s">
-        <v>724</v>
+        <v>721</v>
       </c>
       <c r="B138" s="12" t="s">
-        <v>725</v>
+        <v>722</v>
       </c>
       <c r="C138" s="12" t="s">
-        <v>726</v>
+        <v>723</v>
       </c>
       <c r="D138" s="12" t="s">
-        <v>984</v>
+        <v>981</v>
       </c>
       <c r="E138" s="13"/>
     </row>
     <row r="139" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A139" s="17" t="s">
-        <v>998</v>
+        <v>995</v>
       </c>
       <c r="B139" s="17" t="s">
-        <v>995</v>
+        <v>992</v>
       </c>
       <c r="C139" s="18"/>
       <c r="D139" s="19" t="s">
-        <v>999</v>
+        <v>996</v>
       </c>
       <c r="E139" s="20">
         <v>4220</v>
@@ -10531,14 +10531,14 @@
     </row>
     <row r="140" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A140" s="17" t="s">
-        <v>1000</v>
+        <v>997</v>
       </c>
       <c r="B140" s="17" t="s">
-        <v>1001</v>
+        <v>998</v>
       </c>
       <c r="C140" s="18"/>
       <c r="D140" s="19" t="s">
-        <v>1002</v>
+        <v>999</v>
       </c>
       <c r="E140" s="20">
         <v>20300</v>
@@ -10546,14 +10546,14 @@
     </row>
     <row r="141" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A141" s="17" t="s">
-        <v>1003</v>
+        <v>1000</v>
       </c>
       <c r="B141" s="17" t="s">
-        <v>1004</v>
+        <v>1001</v>
       </c>
       <c r="C141" s="18"/>
       <c r="D141" s="19" t="s">
-        <v>1005</v>
+        <v>1002</v>
       </c>
       <c r="E141" s="20">
         <v>2530</v>
@@ -10561,14 +10561,14 @@
     </row>
     <row r="142" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A142" s="17" t="s">
-        <v>1006</v>
+        <v>1003</v>
       </c>
       <c r="B142" s="17" t="s">
-        <v>1007</v>
+        <v>1004</v>
       </c>
       <c r="C142" s="18"/>
       <c r="D142" s="19" t="s">
-        <v>1008</v>
+        <v>1005</v>
       </c>
       <c r="E142" s="20">
         <v>5320</v>
@@ -10576,14 +10576,14 @@
     </row>
     <row r="143" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A143" s="17" t="s">
-        <v>1009</v>
+        <v>1006</v>
       </c>
       <c r="B143" s="17" t="s">
-        <v>1010</v>
+        <v>1007</v>
       </c>
       <c r="C143" s="18"/>
       <c r="D143" s="19" t="s">
-        <v>1011</v>
+        <v>1008</v>
       </c>
       <c r="E143" s="20">
         <v>1070</v>
@@ -10591,14 +10591,14 @@
     </row>
     <row r="144" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A144" s="17" t="s">
-        <v>1012</v>
+        <v>1009</v>
       </c>
       <c r="B144" s="17" t="s">
-        <v>1013</v>
+        <v>1010</v>
       </c>
       <c r="C144" s="18"/>
       <c r="D144" s="19" t="s">
-        <v>1014</v>
+        <v>1011</v>
       </c>
       <c r="E144" s="20">
         <v>3200</v>
@@ -10606,14 +10606,14 @@
     </row>
     <row r="145" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A145" s="17" t="s">
-        <v>993</v>
+        <v>990</v>
       </c>
       <c r="B145" s="17" t="s">
-        <v>994</v>
+        <v>991</v>
       </c>
       <c r="C145" s="18"/>
       <c r="D145" s="19" t="s">
-        <v>1016</v>
+        <v>1013</v>
       </c>
       <c r="E145" s="20">
         <v>2990</v>
@@ -10646,162 +10646,162 @@
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>744</v>
+        <v>741</v>
       </c>
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>745</v>
+        <v>742</v>
       </c>
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>746</v>
+        <v>743</v>
       </c>
     </row>
     <row r="4" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>747</v>
+        <v>744</v>
       </c>
     </row>
     <row r="5" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>748</v>
+        <v>745</v>
       </c>
     </row>
     <row r="6" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>749</v>
+        <v>746</v>
       </c>
     </row>
     <row r="7" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>750</v>
+        <v>747</v>
       </c>
     </row>
     <row r="8" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>751</v>
+        <v>748</v>
       </c>
     </row>
     <row r="9" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>752</v>
+        <v>749</v>
       </c>
     </row>
     <row r="10" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>753</v>
+        <v>750</v>
       </c>
     </row>
     <row r="11" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>754</v>
+        <v>751</v>
       </c>
     </row>
     <row r="12" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>755</v>
+        <v>752</v>
       </c>
     </row>
     <row r="13" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>756</v>
+        <v>753</v>
       </c>
     </row>
     <row r="14" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>757</v>
+        <v>754</v>
       </c>
     </row>
     <row r="15" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>758</v>
+        <v>755</v>
       </c>
     </row>
     <row r="16" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>759</v>
+        <v>756</v>
       </c>
     </row>
     <row r="17" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>760</v>
+        <v>757</v>
       </c>
     </row>
     <row r="18" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>761</v>
+        <v>758</v>
       </c>
     </row>
     <row r="19" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>762</v>
+        <v>759</v>
       </c>
     </row>
     <row r="20" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>763</v>
+        <v>760</v>
       </c>
     </row>
     <row r="21" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>764</v>
+        <v>761</v>
       </c>
     </row>
     <row r="22" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>765</v>
+        <v>762</v>
       </c>
     </row>
     <row r="23" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>766</v>
+        <v>763</v>
       </c>
     </row>
     <row r="24" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>767</v>
+        <v>764</v>
       </c>
     </row>
     <row r="25" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>768</v>
+        <v>765</v>
       </c>
     </row>
     <row r="26" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>769</v>
+        <v>766</v>
       </c>
     </row>
     <row r="27" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>770</v>
+        <v>767</v>
       </c>
     </row>
     <row r="28" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>771</v>
+        <v>768</v>
       </c>
     </row>
     <row r="29" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>772</v>
+        <v>769</v>
       </c>
     </row>
     <row r="30" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>773</v>
+        <v>770</v>
       </c>
     </row>
     <row r="31" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>774</v>
+        <v>771</v>
       </c>
     </row>
     <row r="32" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>775</v>
+        <v>772</v>
       </c>
     </row>
   </sheetData>

</xml_diff>